<commit_message>
Folder cleaning + death data update + icd10_to_CAUSE fix
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/icd10_to_CAUSE.xlsx
+++ b/myCBD/myInfo/icd10_to_CAUSE.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\CCB\CCB Project\0.CCB\myCBD\myInfo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="10935"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -14,8 +19,16 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$1:$Y$226</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -31,7 +44,7 @@
     <author>Dauphine, David (CDPH-CHSI)</author>
   </authors>
   <commentList>
-    <comment ref="L1" authorId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -55,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C58" authorId="1">
+    <comment ref="C58" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P127" authorId="2">
+    <comment ref="P127" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -108,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3097" uniqueCount="1425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3097" uniqueCount="1426">
   <si>
     <t>I. Communicable, maternal, perinatal and nutritional conditions</t>
   </si>
@@ -3747,9 +3760,6 @@
   </si>
   <si>
     <t>K70, K713-K715, K717, K721-K769, I850, I859</t>
-  </si>
-  <si>
-    <t>K70|K71[3-5,7]|K[721-769]|I85[0,9]</t>
   </si>
   <si>
     <t>K713-715, 717, 721-769 to Cirrhosis</t>
@@ -3859,9 +3869,6 @@
     <t>A02, A05, A20-A28, A31, A32, A38, A40-A49, A65-A70, A74-A79, A80-A81, A87-A89, A92-A99, B00-B04, B06-B09, B17.8, B25-B49, B58-B60, B64, B66, B68, B70-B72, B74.3-B74.9, B75, B82-B89, B91-B99 (minus B94.1), G14, M725-726</t>
   </si>
   <si>
-    <t>A0[2,5]|A2[0-8]|A3[1,2,8]|A4|A6[5-9]|A7[0,4-9]|A8[0-1,7-9]|A9[2-9]|B0[0-4,6-9]|B178|B2[5-9]|B3|B4|B5[8-9]|B6[0,4,6,8]|B7[0-2]|B74[3-9]|B75|B8[2-9]|B9[0-3,5-9]|B94[0,2-9]|G14|M72[5-6]</t>
-  </si>
-  <si>
     <t>IHME/CCB</t>
   </si>
   <si>
@@ -4146,9 +4153,6 @@
   </si>
   <si>
     <t>Added I50 from Other cardiovascual diseases</t>
-  </si>
-  <si>
-    <t>Move I271 to Other MSK, I850, I859 to Cirrhosis; I50 to Congestive heart failure</t>
   </si>
   <si>
     <t>IHME; CDPH Programs</t>
@@ -4532,11 +4536,35 @@
   <si>
     <t>U07</t>
   </si>
+  <si>
+    <t>K70|K71[3-5,7]|K72[1-9]|K7[3-6]|I85[0,9]</t>
+  </si>
+  <si>
+    <t>A0[2,5]|A2[0-8]|A3[1,2,8]|A4|A6[5-9]|A7[0,4-9]|A8[0-1,7-9]|A9[2-9]|B0[0-4,6-9]|B178|B2[5-9]|B3|B4|B5[8-9]|B6[0,4,6,8]|B7[0-2]|B74[3-9]|B75|B8[2-9]|B9[1-3,5-9]|B94[0,2-9]|G14|M72[5-6]</t>
+  </si>
+  <si>
+    <t>L[0-8]|L9[0-8]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Move I271 to Other MSK, I850, I859 to Cirrhosis; I50 to Congestive heart failure; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>should I00 be moved to infectious disease/strep</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###0.;###0."/>
   </numFmts>
@@ -5221,7 +5249,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5256,7 +5284,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5468,15 +5496,15 @@
   <dimension ref="A1:Y233"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K55" sqref="K55"/>
+      <selection pane="bottomRight" activeCell="A219" sqref="A219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.42578125" style="44" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" style="44" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" style="46" customWidth="1"/>
     <col min="3" max="3" width="35.7109375" style="44" customWidth="1"/>
     <col min="4" max="4" width="4.42578125" style="56" customWidth="1"/>
@@ -5484,7 +5512,7 @@
     <col min="6" max="6" width="5.85546875" style="56" customWidth="1"/>
     <col min="7" max="7" width="8.28515625" style="56" customWidth="1"/>
     <col min="8" max="8" width="8" style="56" customWidth="1"/>
-    <col min="9" max="9" width="62.85546875" style="16" customWidth="1"/>
+    <col min="9" max="9" width="39" style="16" customWidth="1"/>
     <col min="10" max="10" width="10" style="48" customWidth="1"/>
     <col min="11" max="11" width="37.28515625" style="16" customWidth="1"/>
     <col min="12" max="12" width="38.140625" style="16" customWidth="1"/>
@@ -5529,10 +5557,10 @@
         <v>1124</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>384</v>
@@ -5541,10 +5569,10 @@
         <v>759</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>1331</v>
+        <v>1328</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>1332</v>
+        <v>1329</v>
       </c>
       <c r="O1" s="59" t="s">
         <v>1160</v>
@@ -5565,7 +5593,7 @@
         <v>878</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>1418</v>
+        <v>1415</v>
       </c>
       <c r="V1" s="20" t="s">
         <v>762</v>
@@ -5885,7 +5913,7 @@
         <v>1154</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="V7" s="20"/>
       <c r="W7" s="2" t="s">
@@ -6134,10 +6162,10 @@
         <v>1047</v>
       </c>
       <c r="T11" s="5" t="s">
-        <v>1401</v>
+        <v>1398</v>
       </c>
       <c r="U11" s="5" t="s">
-        <v>1401</v>
+        <v>1398</v>
       </c>
       <c r="V11" s="20" t="s">
         <v>6</v>
@@ -6506,10 +6534,10 @@
         <v>1059</v>
       </c>
       <c r="T17" s="5" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
       <c r="U17" s="5" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
       <c r="V17" s="20" t="s">
         <v>10</v>
@@ -8479,16 +8507,16 @@
       </c>
       <c r="H51" s="40"/>
       <c r="I51" s="5" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="L51" s="19" t="s">
-        <v>1230</v>
+        <v>1423</v>
       </c>
       <c r="M51" s="19"/>
       <c r="N51" s="19"/>
@@ -8521,7 +8549,7 @@
         <v>880</v>
       </c>
       <c r="Y51" s="5" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.25">
@@ -8621,13 +8649,13 @@
         <v>404</v>
       </c>
       <c r="L53" s="75" t="s">
-        <v>1327</v>
+        <v>1324</v>
       </c>
       <c r="M53" s="75" t="s">
-        <v>1352</v>
+        <v>1349</v>
       </c>
       <c r="N53" s="75" t="s">
-        <v>1353</v>
+        <v>1350</v>
       </c>
       <c r="O53" s="59" t="s">
         <v>404</v>
@@ -8738,7 +8766,7 @@
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="31" t="s">
-        <v>1422</v>
+        <v>1419</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>1136</v>
@@ -8758,10 +8786,10 @@
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
       <c r="K55" s="5" t="s">
-        <v>1423</v>
+        <v>1420</v>
       </c>
       <c r="L55" s="16" t="s">
-        <v>1424</v>
+        <v>1421</v>
       </c>
       <c r="O55" s="59"/>
       <c r="P55" s="60"/>
@@ -8769,7 +8797,7 @@
       <c r="R55" s="83"/>
       <c r="S55" s="83"/>
       <c r="T55" s="5" t="s">
-        <v>1422</v>
+        <v>1419</v>
       </c>
       <c r="U55" s="5"/>
       <c r="V55" s="20"/>
@@ -8935,16 +8963,16 @@
       <c r="I58" s="5"/>
       <c r="J58" s="5"/>
       <c r="K58" s="5" t="s">
-        <v>1354</v>
+        <v>1351</v>
       </c>
       <c r="L58" s="16" t="s">
-        <v>1363</v>
+        <v>1360</v>
       </c>
       <c r="M58" s="16" t="s">
-        <v>1355</v>
+        <v>1352</v>
       </c>
       <c r="N58" s="16" t="s">
-        <v>1363</v>
+        <v>1360</v>
       </c>
       <c r="O58" s="59" t="s">
         <v>408</v>
@@ -8960,10 +8988,10 @@
         <v>1066</v>
       </c>
       <c r="T58" s="5" t="s">
-        <v>1403</v>
+        <v>1400</v>
       </c>
       <c r="U58" s="5" t="s">
-        <v>1403</v>
+        <v>1400</v>
       </c>
       <c r="V58" s="20" t="s">
         <v>33</v>
@@ -8975,7 +9003,7 @@
         <v>33</v>
       </c>
       <c r="Y58" s="5" t="s">
-        <v>1356</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.25">
@@ -9077,7 +9105,7 @@
         <v>370</v>
       </c>
       <c r="M60" s="16" t="s">
-        <v>1357</v>
+        <v>1354</v>
       </c>
       <c r="N60" s="16" t="s">
         <v>370</v>
@@ -9111,7 +9139,7 @@
         <v>35</v>
       </c>
       <c r="Y60" s="5" t="s">
-        <v>1358</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.25">
@@ -9165,10 +9193,10 @@
         <v>1065</v>
       </c>
       <c r="T61" s="5" t="s">
-        <v>1412</v>
+        <v>1409</v>
       </c>
       <c r="U61" s="5" t="s">
-        <v>1412</v>
+        <v>1409</v>
       </c>
       <c r="V61" s="20" t="s">
         <v>36</v>
@@ -9213,10 +9241,10 @@
         <v>372</v>
       </c>
       <c r="M62" s="16" t="s">
-        <v>1359</v>
+        <v>1356</v>
       </c>
       <c r="N62" s="16" t="s">
-        <v>1360</v>
+        <v>1357</v>
       </c>
       <c r="O62" s="59" t="s">
         <v>412</v>
@@ -9280,10 +9308,10 @@
         <v>373</v>
       </c>
       <c r="M63" s="16" t="s">
-        <v>1361</v>
+        <v>1358</v>
       </c>
       <c r="N63" s="16" t="s">
-        <v>1362</v>
+        <v>1359</v>
       </c>
       <c r="O63" s="59" t="s">
         <v>413</v>
@@ -9587,7 +9615,7 @@
       </c>
       <c r="H68" s="40"/>
       <c r="I68" s="5" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="J68" s="5" t="s">
         <v>1159</v>
@@ -9596,7 +9624,7 @@
         <v>1164</v>
       </c>
       <c r="L68" s="19" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="M68" s="19"/>
       <c r="N68" s="19"/>
@@ -9717,7 +9745,7 @@
         <v>420</v>
       </c>
       <c r="L70" s="16" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="O70" s="59" t="s">
         <v>420</v>
@@ -9912,10 +9940,10 @@
         <v>1033</v>
       </c>
       <c r="T73" s="5" t="s">
-        <v>1413</v>
+        <v>1410</v>
       </c>
       <c r="U73" s="5" t="s">
-        <v>1413</v>
+        <v>1410</v>
       </c>
       <c r="V73" s="20" t="s">
         <v>48</v>
@@ -10023,7 +10051,7 @@
       </c>
       <c r="Q75" s="59"/>
       <c r="R75" s="86" t="s">
-        <v>1387</v>
+        <v>1384</v>
       </c>
       <c r="S75" s="83" t="s">
         <v>557</v>
@@ -10131,10 +10159,10 @@
         <v>558</v>
       </c>
       <c r="T77" s="2" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="U77" s="2" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="V77" s="20" t="s">
         <v>51</v>
@@ -10176,10 +10204,10 @@
       <c r="I78" s="5"/>
       <c r="J78" s="5"/>
       <c r="K78" s="5" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="L78" s="49" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="M78" s="49"/>
       <c r="N78" s="49"/>
@@ -10233,16 +10261,16 @@
       </c>
       <c r="H79" s="40"/>
       <c r="I79" s="18" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="J79" s="17" t="s">
         <v>1159</v>
       </c>
       <c r="K79" s="5" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="L79" s="19" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="M79" s="19"/>
       <c r="N79" s="19"/>
@@ -10300,7 +10328,7 @@
       </c>
       <c r="H80" s="40"/>
       <c r="I80" s="19" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="J80" s="17" t="s">
         <v>1159</v>
@@ -10327,10 +10355,10 @@
         <v>1087</v>
       </c>
       <c r="T80" s="5" t="s">
-        <v>1414</v>
+        <v>1411</v>
       </c>
       <c r="U80" s="5" t="s">
-        <v>1414</v>
+        <v>1411</v>
       </c>
       <c r="V80" s="50" t="s">
         <v>896</v>
@@ -10433,7 +10461,7 @@
         <v>B02</v>
       </c>
       <c r="I82" s="18" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="J82" s="17" t="s">
         <v>1159</v>
@@ -10460,10 +10488,10 @@
         <v>1089</v>
       </c>
       <c r="T82" s="5" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="U82" s="5" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="V82" s="50" t="s">
         <v>53</v>
@@ -10503,7 +10531,7 @@
         <v>B03</v>
       </c>
       <c r="I83" s="18" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="J83" s="17" t="s">
         <v>1159</v>
@@ -10575,16 +10603,16 @@
         <v>B04</v>
       </c>
       <c r="I84" s="16" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="J84" s="17" t="s">
         <v>1159</v>
       </c>
       <c r="K84" s="5" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="L84" s="49" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="M84" s="49"/>
       <c r="N84" s="49"/>
@@ -10645,7 +10673,7 @@
         <v>B05</v>
       </c>
       <c r="I85" s="18" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="J85" s="17" t="s">
         <v>1159</v>
@@ -10715,7 +10743,7 @@
         <v>B06</v>
       </c>
       <c r="I86" s="18" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="J86" s="17" t="s">
         <v>1159</v>
@@ -10785,7 +10813,7 @@
         <v>B07</v>
       </c>
       <c r="I87" s="18" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="J87" s="17" t="s">
         <v>1159</v>
@@ -10815,7 +10843,7 @@
         <v>221</v>
       </c>
       <c r="U87" s="5" t="s">
-        <v>1421</v>
+        <v>1418</v>
       </c>
       <c r="V87" s="50" t="s">
         <v>58</v>
@@ -10914,16 +10942,16 @@
       </c>
       <c r="H89" s="40"/>
       <c r="I89" s="18" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="J89" s="17" t="s">
         <v>1159</v>
       </c>
       <c r="K89" s="5" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="L89" s="49" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="M89" s="49"/>
       <c r="N89" s="49"/>
@@ -10981,16 +11009,16 @@
       </c>
       <c r="H90" s="40"/>
       <c r="I90" s="18" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="J90" s="17" t="s">
         <v>1159</v>
       </c>
       <c r="K90" s="5" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="L90" s="49" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="M90" s="49"/>
       <c r="N90" s="49"/>
@@ -11051,7 +11079,7 @@
         <v>B09</v>
       </c>
       <c r="I91" s="16" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="J91" s="17" t="s">
         <v>1159</v>
@@ -11101,7 +11129,7 @@
       </c>
       <c r="B92" s="2"/>
       <c r="C92" s="37" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="D92" s="6" t="s">
         <v>1137</v>
@@ -11128,14 +11156,14 @@
       <c r="R92" s="83"/>
       <c r="S92" s="83"/>
       <c r="T92" s="5" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="U92" s="5" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="V92" s="20"/>
       <c r="W92" s="5" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="X92" s="45"/>
       <c r="Y92" s="2"/>
@@ -11164,7 +11192,7 @@
       </c>
       <c r="H93" s="40"/>
       <c r="I93" s="5" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="J93" s="17" t="s">
         <v>1159</v>
@@ -11231,16 +11259,16 @@
       </c>
       <c r="H94" s="40"/>
       <c r="I94" s="5" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="J94" s="17" t="s">
         <v>1159</v>
       </c>
       <c r="K94" s="5" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="L94" s="49" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="M94" s="49"/>
       <c r="N94" s="49"/>
@@ -11301,16 +11329,16 @@
         <v>B11</v>
       </c>
       <c r="I95" s="5" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="J95" s="17" t="s">
         <v>1159</v>
       </c>
       <c r="K95" s="5" t="s">
+        <v>1204</v>
+      </c>
+      <c r="L95" s="49" t="s">
         <v>1205</v>
-      </c>
-      <c r="L95" s="49" t="s">
-        <v>1206</v>
       </c>
       <c r="M95" s="49"/>
       <c r="N95" s="49"/>
@@ -11371,7 +11399,7 @@
         <v>B12</v>
       </c>
       <c r="I96" s="19" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="J96" s="17" t="s">
         <v>1159</v>
@@ -11438,7 +11466,7 @@
       </c>
       <c r="H97" s="40"/>
       <c r="I97" s="19" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="J97" s="17" t="s">
         <v>1159</v>
@@ -11508,16 +11536,16 @@
         <v>B13</v>
       </c>
       <c r="I98" s="19" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="J98" s="17" t="s">
         <v>1159</v>
       </c>
       <c r="K98" s="5" t="s">
+        <v>1206</v>
+      </c>
+      <c r="L98" s="49" t="s">
         <v>1207</v>
-      </c>
-      <c r="L98" s="49" t="s">
-        <v>1208</v>
       </c>
       <c r="M98" s="49"/>
       <c r="N98" s="49"/>
@@ -11578,16 +11606,16 @@
         <v>B14</v>
       </c>
       <c r="I99" s="5" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="J99" s="17" t="s">
         <v>1159</v>
       </c>
       <c r="K99" s="5" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="L99" s="49" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="M99" s="49"/>
       <c r="N99" s="49"/>
@@ -11648,7 +11676,7 @@
         <v>B15</v>
       </c>
       <c r="I100" s="16" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="J100" s="17" t="s">
         <v>1159</v>
@@ -11715,7 +11743,7 @@
       </c>
       <c r="H101" s="40"/>
       <c r="I101" s="19" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="J101" s="17" t="s">
         <v>1159</v>
@@ -11742,10 +11770,10 @@
         <v>1075</v>
       </c>
       <c r="T101" s="5" t="s">
-        <v>1415</v>
+        <v>1412</v>
       </c>
       <c r="U101" s="5" t="s">
-        <v>1415</v>
+        <v>1412</v>
       </c>
       <c r="V101" s="20" t="s">
         <v>707</v>
@@ -11782,7 +11810,7 @@
       </c>
       <c r="H102" s="40"/>
       <c r="I102" s="19" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="J102" s="17" t="s">
         <v>1159</v>
@@ -11849,7 +11877,7 @@
       </c>
       <c r="H103" s="40"/>
       <c r="I103" s="19" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="J103" s="17" t="s">
         <v>1159</v>
@@ -12272,10 +12300,10 @@
         <v>1030</v>
       </c>
       <c r="T109" s="5" t="s">
-        <v>1405</v>
+        <v>1402</v>
       </c>
       <c r="U109" s="5" t="s">
-        <v>1405</v>
+        <v>1402</v>
       </c>
       <c r="V109" s="20" t="s">
         <v>715</v>
@@ -12315,16 +12343,16 @@
         <v>B99</v>
       </c>
       <c r="I110" s="5" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="J110" s="5" t="s">
         <v>1159</v>
       </c>
       <c r="K110" s="5" t="s">
+        <v>1208</v>
+      </c>
+      <c r="L110" s="49" t="s">
         <v>1209</v>
-      </c>
-      <c r="L110" s="49" t="s">
-        <v>1210</v>
       </c>
       <c r="M110" s="49"/>
       <c r="N110" s="49"/>
@@ -12378,10 +12406,10 @@
       </c>
       <c r="H111" s="40"/>
       <c r="K111" s="5" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="L111" s="5" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="M111" s="5"/>
       <c r="N111" s="5"/>
@@ -12442,22 +12470,22 @@
         <v>D01</v>
       </c>
       <c r="I112" s="5" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="J112" s="5" t="s">
         <v>1159</v>
       </c>
       <c r="K112" s="5" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="L112" s="49" t="s">
+        <v>1327</v>
+      </c>
+      <c r="M112" s="49" t="s">
+        <v>1332</v>
+      </c>
+      <c r="N112" s="49" t="s">
         <v>1330</v>
-      </c>
-      <c r="M112" s="49" t="s">
-        <v>1335</v>
-      </c>
-      <c r="N112" s="49" t="s">
-        <v>1333</v>
       </c>
       <c r="O112" s="59" t="s">
         <v>975</v>
@@ -12488,7 +12516,7 @@
         <v>66</v>
       </c>
       <c r="Y112" s="2" t="s">
-        <v>1334</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="113" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
@@ -12519,18 +12547,18 @@
       <c r="I113" s="5"/>
       <c r="J113" s="5"/>
       <c r="K113" s="5" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="L113" s="19" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="M113" s="19"/>
       <c r="N113" s="19"/>
       <c r="O113" s="59" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="P113" s="62" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="Q113" s="65"/>
       <c r="R113" s="83" t="s">
@@ -12732,10 +12760,10 @@
         <v>1105</v>
       </c>
       <c r="T116" s="5" t="s">
-        <v>1416</v>
+        <v>1413</v>
       </c>
       <c r="U116" s="5" t="s">
-        <v>1416</v>
+        <v>1413</v>
       </c>
       <c r="V116" s="5" t="s">
         <v>719</v>
@@ -12880,7 +12908,7 @@
       </c>
       <c r="B119" s="2"/>
       <c r="C119" s="32" t="s">
-        <v>1345</v>
+        <v>1342</v>
       </c>
       <c r="D119" s="6" t="s">
         <v>1140</v>
@@ -12908,14 +12936,14 @@
       <c r="R119" s="83"/>
       <c r="S119" s="83"/>
       <c r="T119" s="2" t="s">
-        <v>1347</v>
+        <v>1344</v>
       </c>
       <c r="U119" s="2" t="s">
-        <v>1347</v>
+        <v>1344</v>
       </c>
       <c r="V119" s="20"/>
       <c r="W119" s="2" t="s">
-        <v>1346</v>
+        <v>1343</v>
       </c>
       <c r="X119" s="45"/>
       <c r="Y119" s="2"/>
@@ -12927,7 +12955,7 @@
       </c>
       <c r="B120" s="2"/>
       <c r="C120" s="32" t="s">
-        <v>1385</v>
+        <v>1382</v>
       </c>
       <c r="D120" s="6" t="s">
         <v>1140</v>
@@ -12953,10 +12981,10 @@
       <c r="R120" s="83"/>
       <c r="S120" s="83"/>
       <c r="T120" s="2" t="s">
-        <v>1386</v>
+        <v>1383</v>
       </c>
       <c r="U120" s="2" t="s">
-        <v>1386</v>
+        <v>1383</v>
       </c>
       <c r="V120" s="20"/>
       <c r="W120" s="2" t="s">
@@ -13267,13 +13295,13 @@
         <v>443</v>
       </c>
       <c r="L126" s="49" t="s">
-        <v>1336</v>
+        <v>1333</v>
       </c>
       <c r="M126" s="49" t="s">
         <v>443</v>
       </c>
       <c r="N126" s="49" t="s">
-        <v>1336</v>
+        <v>1333</v>
       </c>
       <c r="O126" s="59" t="s">
         <v>443</v>
@@ -13334,24 +13362,24 @@
         <v>D05a</v>
       </c>
       <c r="I127" s="5" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="J127" s="5" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="K127" s="5" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="L127" s="19" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="M127" s="19"/>
       <c r="N127" s="19"/>
       <c r="O127" s="59" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="P127" s="62" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="Q127" s="65"/>
       <c r="R127" s="83" t="s">
@@ -13462,14 +13490,14 @@
         <v>D05b</v>
       </c>
       <c r="I129" s="79" t="s">
-        <v>1382</v>
+        <v>1379</v>
       </c>
       <c r="J129" s="5"/>
       <c r="K129" s="5" t="s">
-        <v>1379</v>
+        <v>1376</v>
       </c>
       <c r="L129" s="49" t="s">
-        <v>1379</v>
+        <v>1376</v>
       </c>
       <c r="M129" s="49"/>
       <c r="N129" s="49"/>
@@ -13721,16 +13749,16 @@
       </c>
       <c r="H133" s="40"/>
       <c r="I133" s="79" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="J133" s="5" t="s">
         <v>1159</v>
       </c>
       <c r="K133" s="5" t="s">
-        <v>1383</v>
+        <v>1380</v>
       </c>
       <c r="L133" s="19" t="s">
-        <v>1384</v>
+        <v>1381</v>
       </c>
       <c r="M133" s="19"/>
       <c r="N133" s="19"/>
@@ -13763,7 +13791,7 @@
         <v>728</v>
       </c>
       <c r="Y133" s="2" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="134" spans="1:25" x14ac:dyDescent="0.25">
@@ -13931,10 +13959,10 @@
       <c r="R136" s="83"/>
       <c r="S136" s="83"/>
       <c r="T136" s="5" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
       <c r="U136" s="5" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
       <c r="V136" s="5" t="s">
         <v>918</v>
@@ -13985,10 +14013,10 @@
       <c r="R137" s="83"/>
       <c r="S137" s="83"/>
       <c r="T137" s="5" t="s">
-        <v>1407</v>
+        <v>1404</v>
       </c>
       <c r="U137" s="5" t="s">
-        <v>1407</v>
+        <v>1404</v>
       </c>
       <c r="V137" s="5" t="s">
         <v>74</v>
@@ -14221,10 +14249,10 @@
       <c r="R141" s="83"/>
       <c r="S141" s="83"/>
       <c r="T141" s="5" t="s">
-        <v>1408</v>
+        <v>1405</v>
       </c>
       <c r="U141" s="5" t="s">
-        <v>1408</v>
+        <v>1405</v>
       </c>
       <c r="V141" s="20" t="s">
         <v>76</v>
@@ -14699,7 +14727,7 @@
         <v>D07</v>
       </c>
       <c r="I149" s="57" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
       <c r="J149" s="18" t="s">
         <v>1159</v>
@@ -14708,7 +14736,7 @@
         <v>1199</v>
       </c>
       <c r="L149" s="58" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
       <c r="M149" s="58"/>
       <c r="N149" s="58"/>
@@ -15065,7 +15093,7 @@
         <v>460</v>
       </c>
       <c r="L155" s="49" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="M155" s="49"/>
       <c r="N155" s="49"/>
@@ -15305,13 +15333,13 @@
         <v>464</v>
       </c>
       <c r="L159" s="49" t="s">
-        <v>826</v>
+        <v>1336</v>
       </c>
       <c r="M159" s="49" t="s">
         <v>464</v>
       </c>
       <c r="N159" s="49" t="s">
-        <v>1339</v>
+        <v>1336</v>
       </c>
       <c r="O159" s="59" t="s">
         <v>464</v>
@@ -15467,10 +15495,10 @@
         <v>1029</v>
       </c>
       <c r="T161" s="5" t="s">
-        <v>1409</v>
+        <v>1406</v>
       </c>
       <c r="U161" s="5" t="s">
-        <v>1409</v>
+        <v>1406</v>
       </c>
       <c r="V161" s="50" t="s">
         <v>96</v>
@@ -15510,22 +15538,22 @@
         <v>C03</v>
       </c>
       <c r="I162" s="5" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="J162" s="5" t="s">
         <v>1159</v>
       </c>
       <c r="K162" s="5" t="s">
+        <v>1224</v>
+      </c>
+      <c r="L162" s="49" t="s">
         <v>1225</v>
       </c>
-      <c r="L162" s="49" t="s">
-        <v>1226</v>
-      </c>
       <c r="M162" s="49" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="N162" s="49" t="s">
-        <v>1340</v>
+        <v>1337</v>
       </c>
       <c r="O162" s="59" t="s">
         <v>467</v>
@@ -15592,10 +15620,10 @@
         <v>830</v>
       </c>
       <c r="M163" s="49" t="s">
-        <v>1337</v>
+        <v>1334</v>
       </c>
       <c r="N163" s="49" t="s">
-        <v>1338</v>
+        <v>1335</v>
       </c>
       <c r="O163" s="59" t="s">
         <v>468</v>
@@ -15626,7 +15654,7 @@
         <v>98</v>
       </c>
       <c r="Y163" s="76" t="s">
-        <v>1344</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="164" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
@@ -15652,22 +15680,22 @@
         <v>C05</v>
       </c>
       <c r="I164" s="5" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="J164" s="5" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="K164" s="5" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="L164" s="49" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="M164" s="49" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="N164" s="49" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="O164" s="59"/>
       <c r="P164" s="64"/>
@@ -15675,17 +15703,17 @@
       <c r="R164" s="83"/>
       <c r="S164" s="83"/>
       <c r="T164" s="5" t="s">
-        <v>1325</v>
+        <v>1322</v>
       </c>
       <c r="U164" s="5" t="s">
-        <v>1325</v>
+        <v>1322</v>
       </c>
       <c r="V164" s="50"/>
       <c r="W164" s="5"/>
       <c r="X164" s="51"/>
       <c r="Y164" s="2"/>
     </row>
-    <row r="165" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:25" ht="51" x14ac:dyDescent="0.25">
       <c r="A165" s="44" t="str">
         <f t="shared" si="13"/>
         <v>...C.99. - Other or unspecified cardiovascular diseases</v>
@@ -15712,22 +15740,22 @@
         <v>C99</v>
       </c>
       <c r="I165" s="5" t="s">
+        <v>1425</v>
+      </c>
+      <c r="J165" s="5" t="s">
+        <v>1319</v>
+      </c>
+      <c r="K165" s="5" t="s">
+        <v>1320</v>
+      </c>
+      <c r="L165" s="19" t="s">
         <v>1321</v>
       </c>
-      <c r="J165" s="5" t="s">
-        <v>1322</v>
-      </c>
-      <c r="K165" s="5" t="s">
-        <v>1323</v>
-      </c>
-      <c r="L165" s="19" t="s">
-        <v>1324</v>
-      </c>
       <c r="M165" s="19" t="s">
-        <v>1342</v>
+        <v>1339</v>
       </c>
       <c r="N165" s="19" t="s">
-        <v>1343</v>
+        <v>1340</v>
       </c>
       <c r="O165" s="59" t="s">
         <v>469</v>
@@ -15743,10 +15771,10 @@
         <v>1102</v>
       </c>
       <c r="T165" s="74" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="U165" s="74" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="V165" s="52" t="s">
         <v>99</v>
@@ -15758,7 +15786,7 @@
         <v>99</v>
       </c>
       <c r="Y165" s="76" t="s">
-        <v>1341</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="166" spans="1:25" x14ac:dyDescent="0.25">
@@ -15836,7 +15864,7 @@
         <v>1140</v>
       </c>
       <c r="E167" s="78" t="s">
-        <v>1349</v>
+        <v>1346</v>
       </c>
       <c r="F167" s="6"/>
       <c r="G167" s="40" t="str">
@@ -15902,7 +15930,7 @@
         <v>1140</v>
       </c>
       <c r="E168" s="78" t="s">
-        <v>1350</v>
+        <v>1347</v>
       </c>
       <c r="F168" s="6"/>
       <c r="G168" s="40" t="str">
@@ -15962,13 +15990,13 @@
         <v>157</v>
       </c>
       <c r="C169" s="31" t="s">
-        <v>1348</v>
+        <v>1345</v>
       </c>
       <c r="D169" s="27" t="s">
         <v>1140</v>
       </c>
       <c r="E169" s="78" t="s">
-        <v>1351</v>
+        <v>1348</v>
       </c>
       <c r="F169" s="6"/>
       <c r="G169" s="40" t="str">
@@ -16068,13 +16096,13 @@
         <v>682</v>
       </c>
       <c r="T170" s="76" t="s">
-        <v>1328</v>
+        <v>1325</v>
       </c>
       <c r="U170" s="76" t="s">
-        <v>1328</v>
+        <v>1325</v>
       </c>
       <c r="V170" s="20" t="s">
-        <v>1329</v>
+        <v>1326</v>
       </c>
       <c r="W170" s="2" t="s">
         <v>281</v>
@@ -16174,7 +16202,7 @@
         <v>D11</v>
       </c>
       <c r="I172" s="16" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="J172" s="5" t="s">
         <v>1159</v>
@@ -16183,7 +16211,7 @@
         <v>1200</v>
       </c>
       <c r="L172" s="49" t="s">
-        <v>1201</v>
+        <v>1422</v>
       </c>
       <c r="M172" s="49"/>
       <c r="N172" s="49"/>
@@ -16619,16 +16647,16 @@
       </c>
       <c r="H179" s="40"/>
       <c r="I179" s="5" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="J179" s="5" t="s">
         <v>1159</v>
       </c>
       <c r="K179" s="5" t="s">
+        <v>1202</v>
+      </c>
+      <c r="L179" s="49" t="s">
         <v>1203</v>
-      </c>
-      <c r="L179" s="49" t="s">
-        <v>1204</v>
       </c>
       <c r="M179" s="49"/>
       <c r="N179" s="49"/>
@@ -16911,10 +16939,10 @@
         <v>2504</v>
       </c>
       <c r="T183" s="5" t="s">
-        <v>1410</v>
+        <v>1407</v>
       </c>
       <c r="U183" s="5" t="s">
-        <v>1410</v>
+        <v>1407</v>
       </c>
       <c r="V183" s="5" t="s">
         <v>928</v>
@@ -17335,7 +17363,7 @@
         <v>483</v>
       </c>
       <c r="L190" s="49" t="s">
-        <v>853</v>
+        <v>1424</v>
       </c>
       <c r="M190" s="49"/>
       <c r="N190" s="49"/>
@@ -17671,7 +17699,7 @@
       </c>
       <c r="Y195" s="2"/>
     </row>
-    <row r="196" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:25" ht="51" x14ac:dyDescent="0.25">
       <c r="A196" s="44" t="str">
         <f t="shared" si="13"/>
         <v/>
@@ -17695,10 +17723,10 @@
       </c>
       <c r="H196" s="40"/>
       <c r="I196" s="5" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="J196" s="5" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="K196" s="5" t="s">
         <v>1197</v>
@@ -18512,7 +18540,7 @@
       </c>
       <c r="Q209" s="62"/>
       <c r="R209" s="86" t="s">
-        <v>1388</v>
+        <v>1385</v>
       </c>
       <c r="S209" s="83" t="s">
         <v>654</v>
@@ -18621,7 +18649,7 @@
         <v>E01</v>
       </c>
       <c r="I211" s="5" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="J211" s="5" t="s">
         <v>1159</v>
@@ -18671,7 +18699,7 @@
       </c>
       <c r="B212" s="2"/>
       <c r="C212" s="31" t="s">
-        <v>1380</v>
+        <v>1377</v>
       </c>
       <c r="D212" s="6" t="s">
         <v>1141</v>
@@ -18693,10 +18721,10 @@
       </c>
       <c r="J212" s="5"/>
       <c r="K212" s="79" t="s">
-        <v>1398</v>
+        <v>1395</v>
       </c>
       <c r="L212" s="80" t="s">
-        <v>1417</v>
+        <v>1414</v>
       </c>
       <c r="M212" s="19"/>
       <c r="N212" s="19"/>
@@ -18706,10 +18734,10 @@
       <c r="R212" s="83"/>
       <c r="S212" s="83"/>
       <c r="T212" s="5" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="U212" s="5" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="V212" s="20"/>
       <c r="W212" s="5"/>
@@ -18725,7 +18753,7 @@
         <v>200</v>
       </c>
       <c r="C213" s="31" t="s">
-        <v>1381</v>
+        <v>1378</v>
       </c>
       <c r="D213" s="6" t="s">
         <v>1141</v>
@@ -18744,13 +18772,13 @@
       </c>
       <c r="I213" s="5"/>
       <c r="J213" s="5" t="s">
+        <v>1394</v>
+      </c>
+      <c r="K213" s="79" t="s">
+        <v>1396</v>
+      </c>
+      <c r="L213" s="81" t="s">
         <v>1397</v>
-      </c>
-      <c r="K213" s="79" t="s">
-        <v>1399</v>
-      </c>
-      <c r="L213" s="81" t="s">
-        <v>1400</v>
       </c>
       <c r="M213" s="49"/>
       <c r="N213" s="49"/>
@@ -18768,10 +18796,10 @@
         <v>1006</v>
       </c>
       <c r="T213" s="5" t="s">
-        <v>1396</v>
+        <v>1393</v>
       </c>
       <c r="U213" s="5" t="s">
-        <v>1396</v>
+        <v>1393</v>
       </c>
       <c r="V213" s="20" t="s">
         <v>135</v>
@@ -19002,10 +19030,10 @@
       <c r="I217" s="5"/>
       <c r="J217" s="5"/>
       <c r="K217" s="5" t="s">
-        <v>1376</v>
+        <v>1373</v>
       </c>
       <c r="L217" s="49" t="s">
-        <v>1378</v>
+        <v>1375</v>
       </c>
       <c r="M217" s="49"/>
       <c r="N217" s="49"/>
@@ -19046,7 +19074,7 @@
       </c>
       <c r="B218" s="2"/>
       <c r="C218" s="31" t="s">
-        <v>1377</v>
+        <v>1374</v>
       </c>
       <c r="D218" s="6" t="s">
         <v>1141</v>
@@ -19061,16 +19089,16 @@
       </c>
       <c r="H218" s="40"/>
       <c r="I218" s="5" t="s">
-        <v>1375</v>
+        <v>1372</v>
       </c>
       <c r="J218" s="5" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="K218" s="5" t="s">
-        <v>1372</v>
+        <v>1369</v>
       </c>
       <c r="L218" s="49" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
       <c r="M218" s="49"/>
       <c r="N218" s="49"/>
@@ -19080,10 +19108,10 @@
       <c r="R218" s="83"/>
       <c r="S218" s="83"/>
       <c r="T218" s="5" t="s">
-        <v>1374</v>
+        <v>1371</v>
       </c>
       <c r="U218" s="5" t="s">
-        <v>1374</v>
+        <v>1371</v>
       </c>
       <c r="V218" s="20"/>
       <c r="W218" s="5"/>
@@ -19114,7 +19142,7 @@
       </c>
       <c r="H219" s="40"/>
       <c r="I219" s="5" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="J219" s="5" t="s">
         <v>1159</v>
@@ -19180,16 +19208,16 @@
         <v>E05</v>
       </c>
       <c r="I220" s="5" t="s">
-        <v>1392</v>
+        <v>1389</v>
       </c>
       <c r="J220" s="5" t="s">
+        <v>1251</v>
+      </c>
+      <c r="K220" s="5" t="s">
+        <v>1252</v>
+      </c>
+      <c r="L220" s="49" t="s">
         <v>1253</v>
-      </c>
-      <c r="K220" s="5" t="s">
-        <v>1254</v>
-      </c>
-      <c r="L220" s="49" t="s">
-        <v>1255</v>
       </c>
       <c r="M220" s="49"/>
       <c r="N220" s="49"/>
@@ -19222,7 +19250,7 @@
         <v>887</v>
       </c>
       <c r="Y220" s="22" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="221" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
@@ -19308,16 +19336,16 @@
         <v>E07</v>
       </c>
       <c r="I222" s="5" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="J222" s="5" t="s">
+        <v>1210</v>
+      </c>
+      <c r="K222" s="5" t="s">
         <v>1211</v>
       </c>
-      <c r="K222" s="5" t="s">
+      <c r="L222" s="49" t="s">
         <v>1212</v>
-      </c>
-      <c r="L222" s="49" t="s">
-        <v>1213</v>
       </c>
       <c r="M222" s="49"/>
       <c r="N222" s="49"/>
@@ -19335,10 +19363,10 @@
         <v>999</v>
       </c>
       <c r="T222" s="5" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="U222" s="5" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="V222" s="20" t="s">
         <v>140</v>
@@ -19378,7 +19406,7 @@
       </c>
       <c r="I223" s="5"/>
       <c r="J223" s="5" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="M223" s="19"/>
       <c r="N223" s="19"/>
@@ -19396,10 +19424,10 @@
         <v>998</v>
       </c>
       <c r="T223" s="5" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="U223" s="5" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="V223" s="20" t="s">
         <v>141</v>
@@ -19437,14 +19465,14 @@
         <v>E08a</v>
       </c>
       <c r="I224" s="5" t="s">
-        <v>1389</v>
+        <v>1386</v>
       </c>
       <c r="J224" s="5"/>
       <c r="K224" s="5" t="s">
+        <v>1364</v>
+      </c>
+      <c r="L224" s="19" t="s">
         <v>1367</v>
-      </c>
-      <c r="L224" s="19" t="s">
-        <v>1370</v>
       </c>
       <c r="M224" s="19"/>
       <c r="N224" s="19"/>
@@ -19454,10 +19482,10 @@
       <c r="R224" s="83"/>
       <c r="S224" s="83"/>
       <c r="T224" s="20" t="s">
-        <v>1365</v>
+        <v>1362</v>
       </c>
       <c r="U224" s="20" t="s">
-        <v>1365</v>
+        <v>1362</v>
       </c>
       <c r="V224" s="46"/>
       <c r="W224" s="5"/>
@@ -19489,16 +19517,16 @@
         <v>E08b</v>
       </c>
       <c r="I225" s="5" t="s">
-        <v>1390</v>
+        <v>1387</v>
       </c>
       <c r="J225" s="5" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="K225" s="5" t="s">
-        <v>1366</v>
+        <v>1363</v>
       </c>
       <c r="L225" s="19" t="s">
-        <v>1371</v>
+        <v>1368</v>
       </c>
       <c r="M225" s="19"/>
       <c r="N225" s="19"/>
@@ -19508,10 +19536,10 @@
       <c r="R225" s="83"/>
       <c r="S225" s="83"/>
       <c r="T225" s="20" t="s">
-        <v>1364</v>
+        <v>1361</v>
       </c>
       <c r="U225" s="20" t="s">
-        <v>1364</v>
+        <v>1361</v>
       </c>
       <c r="V225" s="46"/>
       <c r="W225" s="5"/>
@@ -19547,16 +19575,16 @@
         <v>E08c</v>
       </c>
       <c r="I226" s="5" t="s">
-        <v>1391</v>
+        <v>1388</v>
       </c>
       <c r="J226" s="5" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="K226" s="5" t="s">
-        <v>1368</v>
+        <v>1365</v>
       </c>
       <c r="L226" s="49" t="s">
-        <v>1369</v>
+        <v>1366</v>
       </c>
       <c r="M226" s="49"/>
       <c r="N226" s="49"/>
@@ -19570,10 +19598,10 @@
       <c r="R226" s="83"/>
       <c r="S226" s="83"/>
       <c r="T226" s="5" t="s">
-        <v>1411</v>
+        <v>1408</v>
       </c>
       <c r="U226" s="5" t="s">
-        <v>1411</v>
+        <v>1408</v>
       </c>
       <c r="V226" s="20" t="s">
         <v>142</v>
@@ -19585,7 +19613,7 @@
         <v>142</v>
       </c>
       <c r="Y226" s="22" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="227" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
@@ -19594,16 +19622,16 @@
         <v>...E.99. - Injuries of unknown intent (e.g., unintentional or self-harm), including overdoses and deaths by firearm</v>
       </c>
       <c r="B227" s="77" t="s">
-        <v>1394</v>
+        <v>1391</v>
       </c>
       <c r="C227" s="16" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="D227" s="54" t="s">
         <v>1141</v>
       </c>
       <c r="E227" s="55" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="G227" s="40" t="str">
         <f t="shared" si="24"/>
@@ -19614,22 +19642,22 @@
         <v>E99</v>
       </c>
       <c r="I227" s="48" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="J227" s="48" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K227" s="16" t="s">
+        <v>1267</v>
+      </c>
+      <c r="L227" s="16" t="s">
         <v>1268</v>
       </c>
-      <c r="K227" s="16" t="s">
-        <v>1269</v>
-      </c>
-      <c r="L227" s="16" t="s">
-        <v>1270</v>
-      </c>
       <c r="T227" s="48" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="U227" s="48" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="228" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
@@ -19638,7 +19666,7 @@
         <v>...Z.01. - Symptoms, signs and ill-defined conditions, not elsewhere classified</v>
       </c>
       <c r="D228" s="56" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="E228" s="55" t="s">
         <v>1142</v>
@@ -19652,22 +19680,22 @@
         <v>Z01</v>
       </c>
       <c r="I228" s="48" t="s">
+        <v>1219</v>
+      </c>
+      <c r="J228" s="48" t="s">
         <v>1220</v>
       </c>
-      <c r="J228" s="48" t="s">
+      <c r="K228" s="16" t="s">
         <v>1221</v>
       </c>
-      <c r="K228" s="16" t="s">
+      <c r="L228" s="16" t="s">
+        <v>1249</v>
+      </c>
+      <c r="T228" s="48" t="s">
         <v>1222</v>
       </c>
-      <c r="L228" s="16" t="s">
-        <v>1251</v>
-      </c>
-      <c r="T228" s="48" t="s">
-        <v>1223</v>
-      </c>
       <c r="U228" s="48" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="229" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
@@ -19687,22 +19715,22 @@
       </c>
       <c r="H229" s="40"/>
       <c r="I229" s="16" t="s">
-        <v>1326</v>
+        <v>1323</v>
       </c>
       <c r="J229" s="48" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="K229" s="16" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="L229" s="16" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="T229" s="48" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="U229" s="48" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="230" spans="1:25" x14ac:dyDescent="0.25">
@@ -19711,7 +19739,7 @@
         <v>...Z.02. - Unknown/Missing Value</v>
       </c>
       <c r="D230" s="56" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="E230" s="55" t="s">
         <v>1143</v>
@@ -19722,10 +19750,10 @@
         <v>Z02</v>
       </c>
       <c r="T230" s="48" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="U230" s="48" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="231" spans="1:25" x14ac:dyDescent="0.25">
@@ -19734,7 +19762,7 @@
         <v>...Z.03. - Code does not map</v>
       </c>
       <c r="D231" s="56" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="E231" s="55" t="s">
         <v>1144</v>
@@ -19745,13 +19773,13 @@
         <v>Z03</v>
       </c>
       <c r="I231" s="16" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="T231" s="48" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="U231" s="48" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="232" spans="1:25" x14ac:dyDescent="0.25">
@@ -19760,7 +19788,7 @@
         <v>..Z. - Unknown/Missing Value</v>
       </c>
       <c r="D232" s="56" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="G232" s="43"/>
       <c r="H232" s="40" t="str">
@@ -19768,10 +19796,10 @@
         <v>Z</v>
       </c>
       <c r="T232" s="48" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="U232" s="48" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="233" spans="1:25" x14ac:dyDescent="0.25">
@@ -19783,7 +19811,7 @@
         <v>1140</v>
       </c>
       <c r="E233" s="55" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="G233" s="43"/>
       <c r="H233" s="40" t="str">
@@ -19791,10 +19819,10 @@
         <v>D99</v>
       </c>
       <c r="T233" s="48" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="U233" s="48" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
     </row>
   </sheetData>
@@ -20035,24 +20063,24 @@
   <sheetData>
     <row r="11" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="70" t="s">
+        <v>1313</v>
+      </c>
+      <c r="D11" s="71" t="s">
+        <v>1312</v>
+      </c>
+      <c r="E11" s="71" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="72" t="s">
+        <v>1314</v>
+      </c>
+      <c r="D12" s="73" t="s">
         <v>1315</v>
       </c>
-      <c r="D11" s="71" t="s">
-        <v>1314</v>
-      </c>
-      <c r="E11" s="71" t="s">
-        <v>1314</v>
-      </c>
-    </row>
-    <row r="12" spans="3:5" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="72" t="s">
+      <c r="E12" s="73" t="s">
         <v>1316</v>
-      </c>
-      <c r="D12" s="73" t="s">
-        <v>1317</v>
-      </c>
-      <c r="E12" s="73" t="s">
-        <v>1318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more standarization and SOPH prep
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/icd10_to_CAUSE.xlsx
+++ b/myCBD/myInfo/icd10_to_CAUSE.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\CCB\CCB Project\0.CCB\myCBD\myInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A38315-AC94-42C4-B678-4CCF0CA5476D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$1:$Y$226</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,14 +38,14 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Dauphine, David (CDPH-CHSI-PHPRB)</author>
     <author>Matt</author>
     <author>Dauphine, David (CDPH-CHSI)</author>
   </authors>
   <commentList>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -68,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C58" authorId="1" shapeId="0">
+    <comment ref="C58" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -92,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P127" authorId="2" shapeId="0">
+    <comment ref="P127" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -3926,9 +3927,6 @@
     <t>E10-E14 (minus E10.2-E10.29, E11.2-E11.29, E12.2, E13.2-E13.29, E14.2), R730, R739</t>
   </si>
   <si>
-    <t>H3[0-2,4-5]|H35[0-2,4-9]|H5[3-4]</t>
-  </si>
-  <si>
     <t>R[0-6]|R7[1-2,4-9]|R73[1-8]|R8|R9[0-4,6-9]</t>
   </si>
   <si>
@@ -4560,11 +4558,14 @@
       <t>should I00 be moved to infectious disease/strep</t>
     </r>
   </si>
+  <si>
+    <t>H3[0-4]|\\bH35\\b|H35[0-2,4-9]|H5[3-4]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###0.;###0."/>
   </numFmts>
@@ -5191,7 +5192,7 @@
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5282,6 +5283,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -5317,6 +5335,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5492,14 +5527,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y233"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B137" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A219" sqref="A219"/>
+      <selection pane="bottomRight" activeCell="L155" sqref="L155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5557,10 +5592,10 @@
         <v>1124</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>384</v>
@@ -5569,10 +5604,10 @@
         <v>759</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>1327</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>1328</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>1329</v>
       </c>
       <c r="O1" s="59" t="s">
         <v>1160</v>
@@ -5593,7 +5628,7 @@
         <v>878</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="V1" s="20" t="s">
         <v>762</v>
@@ -5913,7 +5948,7 @@
         <v>1154</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="V7" s="20"/>
       <c r="W7" s="2" t="s">
@@ -6162,10 +6197,10 @@
         <v>1047</v>
       </c>
       <c r="T11" s="5" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="U11" s="5" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="V11" s="20" t="s">
         <v>6</v>
@@ -6534,10 +6569,10 @@
         <v>1059</v>
       </c>
       <c r="T17" s="5" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="U17" s="5" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="V17" s="20" t="s">
         <v>10</v>
@@ -6849,7 +6884,7 @@
       </c>
       <c r="Y22" s="2"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A23" s="44" t="str">
         <f t="shared" si="0"/>
         <v>...A.04. - Meningitis</v>
@@ -6913,7 +6948,7 @@
       </c>
       <c r="Y23" s="2"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A24" s="44" t="str">
         <f t="shared" si="0"/>
         <v>...A.05. - Encephalitis</v>
@@ -6977,7 +7012,7 @@
       </c>
       <c r="Y24" s="2"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A25" s="44" t="str">
         <f t="shared" si="0"/>
         <v>...A.06. - Hepatitis</v>
@@ -7091,7 +7126,7 @@
       </c>
       <c r="Y26" s="2"/>
     </row>
-    <row r="27" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="44" t="str">
         <f t="shared" si="0"/>
         <v>....A.06.a. - Acute hepatitis B</v>
@@ -7182,7 +7217,7 @@
       <c r="X28" s="45"/>
       <c r="Y28" s="2"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A29" s="44" t="str">
         <f t="shared" si="0"/>
         <v>....A.06.b. - Acute hepatitis C</v>
@@ -8507,7 +8542,7 @@
       </c>
       <c r="H51" s="40"/>
       <c r="I51" s="5" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="J51" s="5" t="s">
         <v>1229</v>
@@ -8516,7 +8551,7 @@
         <v>1228</v>
       </c>
       <c r="L51" s="19" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="M51" s="19"/>
       <c r="N51" s="19"/>
@@ -8549,10 +8584,10 @@
         <v>880</v>
       </c>
       <c r="Y51" s="5" t="s">
-        <v>1306</v>
-      </c>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A52" s="44" t="str">
         <f t="shared" si="0"/>
         <v>...A.07. - Respiratory infections</v>
@@ -8615,7 +8650,7 @@
       </c>
       <c r="Y52" s="2"/>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A53" s="44" t="str">
         <f t="shared" si="0"/>
         <v>....A.07.a. - Lower respiratory infections</v>
@@ -8649,13 +8684,13 @@
         <v>404</v>
       </c>
       <c r="L53" s="75" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="M53" s="75" t="s">
+        <v>1348</v>
+      </c>
+      <c r="N53" s="75" t="s">
         <v>1349</v>
-      </c>
-      <c r="N53" s="75" t="s">
-        <v>1350</v>
       </c>
       <c r="O53" s="59" t="s">
         <v>404</v>
@@ -8687,7 +8722,7 @@
       </c>
       <c r="Y53" s="2"/>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A54" s="44" t="str">
         <f t="shared" si="0"/>
         <v>....A.07.b. - Upper respiratory infections</v>
@@ -8759,14 +8794,14 @@
       </c>
       <c r="Y54" s="2"/>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A55" s="44" t="str">
         <f t="shared" si="0"/>
         <v>...A.10. - COVID-19</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="31" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>1136</v>
@@ -8786,10 +8821,10 @@
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
       <c r="K55" s="5" t="s">
+        <v>1419</v>
+      </c>
+      <c r="L55" s="16" t="s">
         <v>1420</v>
-      </c>
-      <c r="L55" s="16" t="s">
-        <v>1421</v>
       </c>
       <c r="O55" s="59"/>
       <c r="P55" s="60"/>
@@ -8797,7 +8832,7 @@
       <c r="R55" s="83"/>
       <c r="S55" s="83"/>
       <c r="T55" s="5" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="U55" s="5"/>
       <c r="V55" s="20"/>
@@ -8872,7 +8907,7 @@
       </c>
       <c r="Y56" s="2"/>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A57" s="44" t="str">
         <f t="shared" si="0"/>
         <v>...A.08. - Maternal conditions</v>
@@ -8963,16 +8998,16 @@
       <c r="I58" s="5"/>
       <c r="J58" s="5"/>
       <c r="K58" s="5" t="s">
+        <v>1350</v>
+      </c>
+      <c r="L58" s="16" t="s">
+        <v>1359</v>
+      </c>
+      <c r="M58" s="16" t="s">
         <v>1351</v>
       </c>
-      <c r="L58" s="16" t="s">
-        <v>1360</v>
-      </c>
-      <c r="M58" s="16" t="s">
-        <v>1352</v>
-      </c>
       <c r="N58" s="16" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="O58" s="59" t="s">
         <v>408</v>
@@ -8988,10 +9023,10 @@
         <v>1066</v>
       </c>
       <c r="T58" s="5" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="U58" s="5" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="V58" s="20" t="s">
         <v>33</v>
@@ -9003,7 +9038,7 @@
         <v>33</v>
       </c>
       <c r="Y58" s="5" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.25">
@@ -9105,7 +9140,7 @@
         <v>370</v>
       </c>
       <c r="M60" s="16" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="N60" s="16" t="s">
         <v>370</v>
@@ -9139,7 +9174,7 @@
         <v>35</v>
       </c>
       <c r="Y60" s="5" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.25">
@@ -9193,10 +9228,10 @@
         <v>1065</v>
       </c>
       <c r="T61" s="5" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="U61" s="5" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="V61" s="20" t="s">
         <v>36</v>
@@ -9241,10 +9276,10 @@
         <v>372</v>
       </c>
       <c r="M62" s="16" t="s">
+        <v>1355</v>
+      </c>
+      <c r="N62" s="16" t="s">
         <v>1356</v>
-      </c>
-      <c r="N62" s="16" t="s">
-        <v>1357</v>
       </c>
       <c r="O62" s="59" t="s">
         <v>412</v>
@@ -9308,10 +9343,10 @@
         <v>373</v>
       </c>
       <c r="M63" s="16" t="s">
+        <v>1357</v>
+      </c>
+      <c r="N63" s="16" t="s">
         <v>1358</v>
-      </c>
-      <c r="N63" s="16" t="s">
-        <v>1359</v>
       </c>
       <c r="O63" s="59" t="s">
         <v>413</v>
@@ -9343,7 +9378,7 @@
       </c>
       <c r="Y63" s="2"/>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A64" s="44" t="str">
         <f t="shared" si="0"/>
         <v>...A.09. - Neonatal conditions</v>
@@ -9591,7 +9626,7 @@
       </c>
       <c r="Y67" s="2"/>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A68" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -9615,7 +9650,7 @@
       </c>
       <c r="H68" s="40"/>
       <c r="I68" s="5" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="J68" s="5" t="s">
         <v>1159</v>
@@ -9940,10 +9975,10 @@
         <v>1033</v>
       </c>
       <c r="T73" s="5" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="U73" s="5" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="V73" s="20" t="s">
         <v>48</v>
@@ -10051,7 +10086,7 @@
       </c>
       <c r="Q75" s="59"/>
       <c r="R75" s="86" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="S75" s="83" t="s">
         <v>557</v>
@@ -10073,7 +10108,7 @@
       </c>
       <c r="Y75" s="2"/>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A76" s="44" t="str">
         <f t="shared" si="6"/>
         <v>..D. - Other Chronic</v>
@@ -10114,7 +10149,7 @@
       </c>
       <c r="Y76" s="2"/>
     </row>
-    <row r="77" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A77" s="44" t="str">
         <f t="shared" si="6"/>
         <v>..B. - Cancer/Malignant neoplasms</v>
@@ -10159,10 +10194,10 @@
         <v>558</v>
       </c>
       <c r="T77" s="2" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="U77" s="2" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="V77" s="20" t="s">
         <v>51</v>
@@ -10175,7 +10210,7 @@
       </c>
       <c r="Y77" s="2"/>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A78" s="44" t="str">
         <f t="shared" si="6"/>
         <v>...B.01. - Mouth and oropharynx cancers</v>
@@ -10204,10 +10239,10 @@
       <c r="I78" s="5"/>
       <c r="J78" s="5"/>
       <c r="K78" s="5" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="L78" s="49" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="M78" s="49"/>
       <c r="N78" s="49"/>
@@ -10237,7 +10272,7 @@
       </c>
       <c r="Y78" s="2"/>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A79" s="44" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -10261,16 +10296,16 @@
       </c>
       <c r="H79" s="40"/>
       <c r="I79" s="18" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="J79" s="17" t="s">
         <v>1159</v>
       </c>
       <c r="K79" s="5" t="s">
+        <v>1261</v>
+      </c>
+      <c r="L79" s="19" t="s">
         <v>1262</v>
-      </c>
-      <c r="L79" s="19" t="s">
-        <v>1263</v>
       </c>
       <c r="M79" s="19"/>
       <c r="N79" s="19"/>
@@ -10328,7 +10363,7 @@
       </c>
       <c r="H80" s="40"/>
       <c r="I80" s="19" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="J80" s="17" t="s">
         <v>1159</v>
@@ -10355,10 +10390,10 @@
         <v>1087</v>
       </c>
       <c r="T80" s="5" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="U80" s="5" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="V80" s="50" t="s">
         <v>896</v>
@@ -10434,7 +10469,7 @@
       </c>
       <c r="Y81" s="2"/>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A82" s="44" t="str">
         <f t="shared" si="6"/>
         <v>...B.02. - Esophagus cancer</v>
@@ -10461,7 +10496,7 @@
         <v>B02</v>
       </c>
       <c r="I82" s="18" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="J82" s="17" t="s">
         <v>1159</v>
@@ -10488,10 +10523,10 @@
         <v>1089</v>
       </c>
       <c r="T82" s="5" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="U82" s="5" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="V82" s="50" t="s">
         <v>53</v>
@@ -10504,7 +10539,7 @@
       </c>
       <c r="Y82" s="2"/>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A83" s="44" t="str">
         <f t="shared" si="6"/>
         <v>...B.03. - Stomach cancer</v>
@@ -10531,7 +10566,7 @@
         <v>B03</v>
       </c>
       <c r="I83" s="18" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="J83" s="17" t="s">
         <v>1159</v>
@@ -10576,7 +10611,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="84" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A84" s="44" t="str">
         <f t="shared" si="6"/>
         <v>...B.04. - Colon and rectum cancers</v>
@@ -10603,7 +10638,7 @@
         <v>B04</v>
       </c>
       <c r="I84" s="16" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="J84" s="17" t="s">
         <v>1159</v>
@@ -10646,7 +10681,7 @@
       </c>
       <c r="Y84" s="2"/>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A85" s="44" t="str">
         <f t="shared" si="6"/>
         <v>...B.05. - Liver cancer</v>
@@ -10673,7 +10708,7 @@
         <v>B05</v>
       </c>
       <c r="I85" s="18" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="J85" s="17" t="s">
         <v>1159</v>
@@ -10716,7 +10751,7 @@
       </c>
       <c r="Y85" s="2"/>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A86" s="44" t="str">
         <f t="shared" si="6"/>
         <v>...B.06. - Pancreas cancer</v>
@@ -10743,7 +10778,7 @@
         <v>B06</v>
       </c>
       <c r="I86" s="18" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="J86" s="17" t="s">
         <v>1159</v>
@@ -10786,7 +10821,7 @@
       </c>
       <c r="Y86" s="2"/>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A87" s="44" t="str">
         <f t="shared" si="6"/>
         <v>...B.07. - Trachea, bronchus and lung cancers</v>
@@ -10813,7 +10848,7 @@
         <v>B07</v>
       </c>
       <c r="I87" s="18" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="J87" s="17" t="s">
         <v>1159</v>
@@ -10843,7 +10878,7 @@
         <v>221</v>
       </c>
       <c r="U87" s="5" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="V87" s="50" t="s">
         <v>58</v>
@@ -10856,7 +10891,7 @@
       </c>
       <c r="Y87" s="2"/>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:25" ht="51" x14ac:dyDescent="0.25">
       <c r="A88" s="44" t="str">
         <f t="shared" si="6"/>
         <v>...B.08. - Melanoma and other skin cancers</v>
@@ -10942,7 +10977,7 @@
       </c>
       <c r="H89" s="40"/>
       <c r="I89" s="18" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="J89" s="17" t="s">
         <v>1159</v>
@@ -11009,7 +11044,7 @@
       </c>
       <c r="H90" s="40"/>
       <c r="I90" s="18" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="J90" s="17" t="s">
         <v>1159</v>
@@ -11052,7 +11087,7 @@
       </c>
       <c r="Y90" s="2"/>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A91" s="44" t="str">
         <f t="shared" si="6"/>
         <v>...B.09. - Breast cancer</v>
@@ -11079,7 +11114,7 @@
         <v>B09</v>
       </c>
       <c r="I91" s="16" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="J91" s="17" t="s">
         <v>1159</v>
@@ -11122,14 +11157,14 @@
       </c>
       <c r="Y91" s="2"/>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A92" s="44" t="str">
         <f t="shared" si="6"/>
         <v>...B.10. - Uterine cancer</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" s="37" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="D92" s="6" t="s">
         <v>1137</v>
@@ -11156,14 +11191,14 @@
       <c r="R92" s="83"/>
       <c r="S92" s="83"/>
       <c r="T92" s="5" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="U92" s="5" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="V92" s="20"/>
       <c r="W92" s="5" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="X92" s="45"/>
       <c r="Y92" s="2"/>
@@ -11192,7 +11227,7 @@
       </c>
       <c r="H93" s="40"/>
       <c r="I93" s="5" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="J93" s="17" t="s">
         <v>1159</v>
@@ -11259,7 +11294,7 @@
       </c>
       <c r="H94" s="40"/>
       <c r="I94" s="5" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="J94" s="17" t="s">
         <v>1159</v>
@@ -11268,7 +11303,7 @@
         <v>1244</v>
       </c>
       <c r="L94" s="49" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="M94" s="49"/>
       <c r="N94" s="49"/>
@@ -11302,7 +11337,7 @@
       </c>
       <c r="Y94" s="2"/>
     </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A95" s="44" t="str">
         <f t="shared" si="6"/>
         <v>...B.11. - Ovary cancer</v>
@@ -11329,7 +11364,7 @@
         <v>B11</v>
       </c>
       <c r="I95" s="5" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="J95" s="17" t="s">
         <v>1159</v>
@@ -11372,7 +11407,7 @@
       </c>
       <c r="Y95" s="2"/>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A96" s="44" t="str">
         <f t="shared" si="6"/>
         <v>...B.12. - Prostate cancer</v>
@@ -11399,7 +11434,7 @@
         <v>B12</v>
       </c>
       <c r="I96" s="19" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="J96" s="17" t="s">
         <v>1159</v>
@@ -11466,7 +11501,7 @@
       </c>
       <c r="H97" s="40"/>
       <c r="I97" s="19" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="J97" s="17" t="s">
         <v>1159</v>
@@ -11509,7 +11544,7 @@
       </c>
       <c r="Y97" s="2"/>
     </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A98" s="44" t="str">
         <f t="shared" si="6"/>
         <v>...B.13. - Kidney, renal pelvis and ureter cancer</v>
@@ -11536,7 +11571,7 @@
         <v>B13</v>
       </c>
       <c r="I98" s="19" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="J98" s="17" t="s">
         <v>1159</v>
@@ -11579,7 +11614,7 @@
       </c>
       <c r="Y98" s="2"/>
     </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A99" s="44" t="str">
         <f t="shared" si="6"/>
         <v>...B.14. - Bladder cancer</v>
@@ -11606,7 +11641,7 @@
         <v>B14</v>
       </c>
       <c r="I99" s="5" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="J99" s="17" t="s">
         <v>1159</v>
@@ -11649,7 +11684,7 @@
       </c>
       <c r="Y99" s="2"/>
     </row>
-    <row r="100" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A100" s="44" t="str">
         <f t="shared" si="6"/>
         <v>...B.15. - Brain and nervous system cancers</v>
@@ -11676,7 +11711,7 @@
         <v>B15</v>
       </c>
       <c r="I100" s="16" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="J100" s="17" t="s">
         <v>1159</v>
@@ -11743,7 +11778,7 @@
       </c>
       <c r="H101" s="40"/>
       <c r="I101" s="19" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="J101" s="17" t="s">
         <v>1159</v>
@@ -11770,10 +11805,10 @@
         <v>1075</v>
       </c>
       <c r="T101" s="5" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="U101" s="5" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="V101" s="20" t="s">
         <v>707</v>
@@ -11810,7 +11845,7 @@
       </c>
       <c r="H102" s="40"/>
       <c r="I102" s="19" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="J102" s="17" t="s">
         <v>1159</v>
@@ -11877,7 +11912,7 @@
       </c>
       <c r="H103" s="40"/>
       <c r="I103" s="19" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="J103" s="17" t="s">
         <v>1159</v>
@@ -11983,7 +12018,7 @@
       </c>
       <c r="Y104" s="2"/>
     </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:25" ht="51" x14ac:dyDescent="0.25">
       <c r="A105" s="44" t="str">
         <f t="shared" si="6"/>
         <v>...B.16. - Lymphomas and multiple myeloma</v>
@@ -12046,7 +12081,7 @@
       </c>
       <c r="Y105" s="2"/>
     </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A106" s="44" t="str">
         <f t="shared" si="6"/>
         <v>....B.16.a. - Hodgkin lymphoma</v>
@@ -12114,7 +12149,7 @@
       </c>
       <c r="Y106" s="2"/>
     </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A107" s="44" t="str">
         <f t="shared" si="6"/>
         <v>....B.16.b. - Non-Hodgkin lymphoma</v>
@@ -12182,7 +12217,7 @@
       </c>
       <c r="Y107" s="2"/>
     </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A108" s="44" t="str">
         <f t="shared" si="6"/>
         <v>....B.16.c. - Multiple myeloma</v>
@@ -12250,7 +12285,7 @@
       </c>
       <c r="Y108" s="2"/>
     </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A109" s="44" t="str">
         <f t="shared" si="6"/>
         <v>...B.17. - Leukemia</v>
@@ -12300,10 +12335,10 @@
         <v>1030</v>
       </c>
       <c r="T109" s="5" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="U109" s="5" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="V109" s="20" t="s">
         <v>715</v>
@@ -12343,7 +12378,7 @@
         <v>B99</v>
       </c>
       <c r="I110" s="5" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="J110" s="5" t="s">
         <v>1159</v>
@@ -12406,10 +12441,10 @@
       </c>
       <c r="H111" s="40"/>
       <c r="K111" s="5" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="L111" s="5" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="M111" s="5"/>
       <c r="N111" s="5"/>
@@ -12470,7 +12505,7 @@
         <v>D01</v>
       </c>
       <c r="I112" s="5" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J112" s="5" t="s">
         <v>1159</v>
@@ -12479,13 +12514,13 @@
         <v>1247</v>
       </c>
       <c r="L112" s="49" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="M112" s="49" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="N112" s="49" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="O112" s="59" t="s">
         <v>975</v>
@@ -12516,10 +12551,10 @@
         <v>66</v>
       </c>
       <c r="Y112" s="2" t="s">
-        <v>1331</v>
-      </c>
-    </row>
-    <row r="113" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="113" spans="1:25" ht="51" x14ac:dyDescent="0.25">
       <c r="A113" s="44" t="str">
         <f t="shared" si="6"/>
         <v>...D.02. - Endocrine, blood, immune disorders</v>
@@ -12547,18 +12582,18 @@
       <c r="I113" s="5"/>
       <c r="J113" s="5"/>
       <c r="K113" s="5" t="s">
+        <v>1301</v>
+      </c>
+      <c r="L113" s="19" t="s">
         <v>1302</v>
-      </c>
-      <c r="L113" s="19" t="s">
-        <v>1303</v>
       </c>
       <c r="M113" s="19"/>
       <c r="N113" s="19"/>
       <c r="O113" s="59" t="s">
+        <v>1301</v>
+      </c>
+      <c r="P113" s="62" t="s">
         <v>1302</v>
-      </c>
-      <c r="P113" s="62" t="s">
-        <v>1303</v>
       </c>
       <c r="Q113" s="65"/>
       <c r="R113" s="83" t="s">
@@ -12647,7 +12682,7 @@
       </c>
       <c r="Y114" s="2"/>
     </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A115" s="44" t="str">
         <f t="shared" si="6"/>
         <v>...D.03. - Sickle cell disorders and trait</v>
@@ -12760,10 +12795,10 @@
         <v>1105</v>
       </c>
       <c r="T116" s="5" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="U116" s="5" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="V116" s="5" t="s">
         <v>719</v>
@@ -12908,7 +12943,7 @@
       </c>
       <c r="B119" s="2"/>
       <c r="C119" s="32" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="D119" s="6" t="s">
         <v>1140</v>
@@ -12936,26 +12971,26 @@
       <c r="R119" s="83"/>
       <c r="S119" s="83"/>
       <c r="T119" s="2" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="U119" s="2" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="V119" s="20"/>
       <c r="W119" s="2" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="X119" s="45"/>
       <c r="Y119" s="2"/>
     </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A120" s="44" t="str">
         <f t="shared" si="6"/>
         <v>...D.05. - Substance use disorders</v>
       </c>
       <c r="B120" s="2"/>
       <c r="C120" s="32" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="D120" s="6" t="s">
         <v>1140</v>
@@ -12981,10 +13016,10 @@
       <c r="R120" s="83"/>
       <c r="S120" s="83"/>
       <c r="T120" s="2" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="U120" s="2" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="V120" s="20"/>
       <c r="W120" s="2" t="s">
@@ -13295,13 +13330,13 @@
         <v>443</v>
       </c>
       <c r="L126" s="49" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="M126" s="49" t="s">
         <v>443</v>
       </c>
       <c r="N126" s="49" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="O126" s="59" t="s">
         <v>443</v>
@@ -13333,7 +13368,7 @@
       </c>
       <c r="Y126" s="2"/>
     </row>
-    <row r="127" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A127" s="44" t="str">
         <f t="shared" si="6"/>
         <v>....D.05.a. - Alcohol use disorders</v>
@@ -13362,7 +13397,7 @@
         <v>D05a</v>
       </c>
       <c r="I127" s="5" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="J127" s="5" t="s">
         <v>1230</v>
@@ -13371,15 +13406,15 @@
         <v>1218</v>
       </c>
       <c r="L127" s="19" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="M127" s="19"/>
       <c r="N127" s="19"/>
       <c r="O127" s="59" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="P127" s="62" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="Q127" s="65"/>
       <c r="R127" s="83" t="s">
@@ -13461,7 +13496,7 @@
       </c>
       <c r="Y128" s="2"/>
     </row>
-    <row r="129" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A129" s="44" t="str">
         <f t="shared" si="6"/>
         <v>....D.05.b. - Opioid use disorders</v>
@@ -13490,14 +13525,14 @@
         <v>D05b</v>
       </c>
       <c r="I129" s="79" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="J129" s="5"/>
       <c r="K129" s="5" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="L129" s="49" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="M129" s="49"/>
       <c r="N129" s="49"/>
@@ -13531,7 +13566,7 @@
       </c>
       <c r="Y129" s="2"/>
     </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A130" s="44" t="str">
         <f t="shared" si="6"/>
         <v>....D.05.c. - Cocaine use disorders</v>
@@ -13599,7 +13634,7 @@
       </c>
       <c r="Y130" s="2"/>
     </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A131" s="44" t="str">
         <f t="shared" si="6"/>
         <v>....D.05.d. - Amphetamine use disorders</v>
@@ -13725,7 +13760,7 @@
       </c>
       <c r="Y132" s="2"/>
     </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A133" s="44" t="str">
         <f t="shared" ref="A133:A196" si="13">IF(H133&lt;&gt;"",IF(F133&lt;&gt;"",CONCATENATE("....",D133,".",E133,".",F133,". - ",T133),IF(E133&lt;&gt;"",CONCATENATE("...",D133,".",E133,". - ",T133),CONCATENATE("..",D133,". - ",T133))),"")</f>
         <v/>
@@ -13749,16 +13784,16 @@
       </c>
       <c r="H133" s="40"/>
       <c r="I133" s="79" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="J133" s="5" t="s">
         <v>1159</v>
       </c>
       <c r="K133" s="5" t="s">
+        <v>1379</v>
+      </c>
+      <c r="L133" s="19" t="s">
         <v>1380</v>
-      </c>
-      <c r="L133" s="19" t="s">
-        <v>1381</v>
       </c>
       <c r="M133" s="19"/>
       <c r="N133" s="19"/>
@@ -13959,10 +13994,10 @@
       <c r="R136" s="83"/>
       <c r="S136" s="83"/>
       <c r="T136" s="5" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="U136" s="5" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="V136" s="5" t="s">
         <v>918</v>
@@ -14013,10 +14048,10 @@
       <c r="R137" s="83"/>
       <c r="S137" s="83"/>
       <c r="T137" s="5" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="U137" s="5" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="V137" s="5" t="s">
         <v>74</v>
@@ -14249,10 +14284,10 @@
       <c r="R141" s="83"/>
       <c r="S141" s="83"/>
       <c r="T141" s="5" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="U141" s="5" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="V141" s="20" t="s">
         <v>76</v>
@@ -14327,7 +14362,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="143" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:25" ht="51" x14ac:dyDescent="0.25">
       <c r="A143" s="44" t="str">
         <f t="shared" si="13"/>
         <v>...D.06. - Alzheimer’s disease and other dementias</v>
@@ -14727,7 +14762,7 @@
         <v>D07</v>
       </c>
       <c r="I149" s="57" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="J149" s="18" t="s">
         <v>1159</v>
@@ -14736,7 +14771,7 @@
         <v>1199</v>
       </c>
       <c r="L149" s="58" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="M149" s="58"/>
       <c r="N149" s="58"/>
@@ -15093,7 +15128,7 @@
         <v>460</v>
       </c>
       <c r="L155" s="49" t="s">
-        <v>1248</v>
+        <v>1425</v>
       </c>
       <c r="M155" s="49"/>
       <c r="N155" s="49"/>
@@ -15333,13 +15368,13 @@
         <v>464</v>
       </c>
       <c r="L159" s="49" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="M159" s="49" t="s">
         <v>464</v>
       </c>
       <c r="N159" s="49" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="O159" s="59" t="s">
         <v>464</v>
@@ -15371,7 +15406,7 @@
       </c>
       <c r="Y159" s="2"/>
     </row>
-    <row r="160" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A160" s="44" t="str">
         <f t="shared" si="13"/>
         <v>...C.01. - Hypertensive heart disease</v>
@@ -15441,7 +15476,7 @@
       </c>
       <c r="Y160" s="2"/>
     </row>
-    <row r="161" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A161" s="44" t="str">
         <f t="shared" si="13"/>
         <v>...C.02. - Ischemic heart disease</v>
@@ -15495,10 +15530,10 @@
         <v>1029</v>
       </c>
       <c r="T161" s="5" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="U161" s="5" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="V161" s="50" t="s">
         <v>96</v>
@@ -15553,7 +15588,7 @@
         <v>1224</v>
       </c>
       <c r="N162" s="49" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="O162" s="59" t="s">
         <v>467</v>
@@ -15585,7 +15620,7 @@
       </c>
       <c r="Y162" s="2"/>
     </row>
-    <row r="163" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:25" ht="51" x14ac:dyDescent="0.25">
       <c r="A163" s="44" t="str">
         <f t="shared" si="13"/>
         <v>...C.04. - Cardiomyopathy, myocarditis, endocarditis</v>
@@ -15620,10 +15655,10 @@
         <v>830</v>
       </c>
       <c r="M163" s="49" t="s">
+        <v>1333</v>
+      </c>
+      <c r="N163" s="49" t="s">
         <v>1334</v>
-      </c>
-      <c r="N163" s="49" t="s">
-        <v>1335</v>
       </c>
       <c r="O163" s="59" t="s">
         <v>468</v>
@@ -15654,10 +15689,10 @@
         <v>98</v>
       </c>
       <c r="Y163" s="76" t="s">
-        <v>1341</v>
-      </c>
-    </row>
-    <row r="164" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="164" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A164" s="44" t="str">
         <f t="shared" si="13"/>
         <v>...C.05. -  Congestive heart failure</v>
@@ -15680,22 +15715,22 @@
         <v>C05</v>
       </c>
       <c r="I164" s="5" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="J164" s="5" t="s">
         <v>1210</v>
       </c>
       <c r="K164" s="5" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="L164" s="49" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="M164" s="49" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="N164" s="49" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="O164" s="59"/>
       <c r="P164" s="64"/>
@@ -15703,10 +15738,10 @@
       <c r="R164" s="83"/>
       <c r="S164" s="83"/>
       <c r="T164" s="5" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="U164" s="5" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="V164" s="50"/>
       <c r="W164" s="5"/>
@@ -15740,22 +15775,22 @@
         <v>C99</v>
       </c>
       <c r="I165" s="5" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="J165" s="5" t="s">
+        <v>1318</v>
+      </c>
+      <c r="K165" s="5" t="s">
         <v>1319</v>
       </c>
-      <c r="K165" s="5" t="s">
+      <c r="L165" s="19" t="s">
         <v>1320</v>
       </c>
-      <c r="L165" s="19" t="s">
-        <v>1321</v>
-      </c>
       <c r="M165" s="19" t="s">
+        <v>1338</v>
+      </c>
+      <c r="N165" s="19" t="s">
         <v>1339</v>
-      </c>
-      <c r="N165" s="19" t="s">
-        <v>1340</v>
       </c>
       <c r="O165" s="59" t="s">
         <v>469</v>
@@ -15771,10 +15806,10 @@
         <v>1102</v>
       </c>
       <c r="T165" s="74" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="U165" s="74" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="V165" s="52" t="s">
         <v>99</v>
@@ -15786,7 +15821,7 @@
         <v>99</v>
       </c>
       <c r="Y165" s="76" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="166" spans="1:25" x14ac:dyDescent="0.25">
@@ -15849,7 +15884,7 @@
       </c>
       <c r="Y166" s="2"/>
     </row>
-    <row r="167" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:25" ht="51" x14ac:dyDescent="0.25">
       <c r="A167" s="44" t="str">
         <f t="shared" si="13"/>
         <v>...D.66. - Chronic obstructive pulmonary disease</v>
@@ -15864,7 +15899,7 @@
         <v>1140</v>
       </c>
       <c r="E167" s="78" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="F167" s="6"/>
       <c r="G167" s="40" t="str">
@@ -15930,7 +15965,7 @@
         <v>1140</v>
       </c>
       <c r="E168" s="78" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="F168" s="6"/>
       <c r="G168" s="40" t="str">
@@ -15981,7 +16016,7 @@
       </c>
       <c r="Y168" s="2"/>
     </row>
-    <row r="169" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A169" s="44" t="str">
         <f t="shared" si="13"/>
         <v>...D.68. - Other respiratory diseases</v>
@@ -15990,13 +16025,13 @@
         <v>157</v>
       </c>
       <c r="C169" s="31" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="D169" s="27" t="s">
         <v>1140</v>
       </c>
       <c r="E169" s="78" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="F169" s="6"/>
       <c r="G169" s="40" t="str">
@@ -16047,7 +16082,7 @@
       </c>
       <c r="Y169" s="2"/>
     </row>
-    <row r="170" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:25" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A170" s="44" t="str">
         <f t="shared" si="13"/>
         <v>...D.09. - Digestive diseases (excluding cirrhosis)</v>
@@ -16096,13 +16131,13 @@
         <v>682</v>
       </c>
       <c r="T170" s="76" t="s">
+        <v>1324</v>
+      </c>
+      <c r="U170" s="76" t="s">
+        <v>1324</v>
+      </c>
+      <c r="V170" s="20" t="s">
         <v>1325</v>
-      </c>
-      <c r="U170" s="76" t="s">
-        <v>1325</v>
-      </c>
-      <c r="V170" s="20" t="s">
-        <v>1326</v>
       </c>
       <c r="W170" s="2" t="s">
         <v>281</v>
@@ -16175,7 +16210,7 @@
       </c>
       <c r="Y171" s="2"/>
     </row>
-    <row r="172" spans="1:25" s="48" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:25" s="48" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A172" s="44" t="str">
         <f t="shared" si="13"/>
         <v>...D.11. - Cirrhosis of the liver</v>
@@ -16211,7 +16246,7 @@
         <v>1200</v>
       </c>
       <c r="L172" s="49" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="M172" s="49"/>
       <c r="N172" s="49"/>
@@ -16748,7 +16783,7 @@
       </c>
       <c r="Y180" s="2"/>
     </row>
-    <row r="181" spans="1:25" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A181" s="44" t="str">
         <f t="shared" si="13"/>
         <v>...D.10. - Kidney diseases</v>
@@ -16815,7 +16850,7 @@
       </c>
       <c r="Y181" s="2"/>
     </row>
-    <row r="182" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A182" s="44" t="str">
         <f t="shared" si="13"/>
         <v>....D.10.a. - Acute glomerulonephritis</v>
@@ -16885,7 +16920,7 @@
       </c>
       <c r="Y182" s="2"/>
     </row>
-    <row r="183" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:25" ht="51" x14ac:dyDescent="0.25">
       <c r="A183" s="44" t="str">
         <f t="shared" si="13"/>
         <v>....D.10.b. - Chronic kidney disease due to diabetes</v>
@@ -16939,10 +16974,10 @@
         <v>2504</v>
       </c>
       <c r="T183" s="5" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="U183" s="5" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="V183" s="5" t="s">
         <v>928</v>
@@ -16955,7 +16990,7 @@
       </c>
       <c r="Y183" s="2"/>
     </row>
-    <row r="184" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A184" s="44" t="str">
         <f t="shared" si="13"/>
         <v>....D.10.c. - Other chronic kidney disease</v>
@@ -17363,7 +17398,7 @@
         <v>483</v>
       </c>
       <c r="L190" s="49" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="M190" s="49"/>
       <c r="N190" s="49"/>
@@ -17723,7 +17758,7 @@
       </c>
       <c r="H196" s="40"/>
       <c r="I196" s="5" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="J196" s="5" t="s">
         <v>1229</v>
@@ -17766,7 +17801,7 @@
       </c>
       <c r="Y196" s="2"/>
     </row>
-    <row r="197" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A197" s="44" t="str">
         <f t="shared" ref="A197:A233" si="20">IF(H197&lt;&gt;"",IF(F197&lt;&gt;"",CONCATENATE("....",D197,".",E197,".",F197,". - ",T197),IF(E197&lt;&gt;"",CONCATENATE("...",D197,".",E197,". - ",T197),CONCATENATE("..",D197,". - ",T197))),"")</f>
         <v>...D.12. - Congenital anomalies</v>
@@ -18540,7 +18575,7 @@
       </c>
       <c r="Q209" s="62"/>
       <c r="R209" s="86" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="S209" s="83" t="s">
         <v>654</v>
@@ -18692,14 +18727,14 @@
       </c>
       <c r="Y211" s="2"/>
     </row>
-    <row r="212" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A212" s="44" t="str">
         <f t="shared" si="20"/>
         <v>...E.02. - Drug poisonings</v>
       </c>
       <c r="B212" s="2"/>
       <c r="C212" s="31" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="D212" s="6" t="s">
         <v>1141</v>
@@ -18721,10 +18756,10 @@
       </c>
       <c r="J212" s="5"/>
       <c r="K212" s="79" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="L212" s="80" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="M212" s="19"/>
       <c r="N212" s="19"/>
@@ -18734,10 +18769,10 @@
       <c r="R212" s="83"/>
       <c r="S212" s="83"/>
       <c r="T212" s="5" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="U212" s="5" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="V212" s="20"/>
       <c r="W212" s="5"/>
@@ -18753,7 +18788,7 @@
         <v>200</v>
       </c>
       <c r="C213" s="31" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="D213" s="6" t="s">
         <v>1141</v>
@@ -18772,13 +18807,13 @@
       </c>
       <c r="I213" s="5"/>
       <c r="J213" s="5" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="K213" s="79" t="s">
+        <v>1395</v>
+      </c>
+      <c r="L213" s="81" t="s">
         <v>1396</v>
-      </c>
-      <c r="L213" s="81" t="s">
-        <v>1397</v>
       </c>
       <c r="M213" s="49"/>
       <c r="N213" s="49"/>
@@ -18796,10 +18831,10 @@
         <v>1006</v>
       </c>
       <c r="T213" s="5" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="U213" s="5" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="V213" s="20" t="s">
         <v>135</v>
@@ -19030,10 +19065,10 @@
       <c r="I217" s="5"/>
       <c r="J217" s="5"/>
       <c r="K217" s="5" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="L217" s="49" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="M217" s="49"/>
       <c r="N217" s="49"/>
@@ -19074,7 +19109,7 @@
       </c>
       <c r="B218" s="2"/>
       <c r="C218" s="31" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="D218" s="6" t="s">
         <v>1141</v>
@@ -19089,16 +19124,16 @@
       </c>
       <c r="H218" s="40"/>
       <c r="I218" s="5" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="J218" s="5" t="s">
         <v>1210</v>
       </c>
       <c r="K218" s="5" t="s">
+        <v>1368</v>
+      </c>
+      <c r="L218" s="49" t="s">
         <v>1369</v>
-      </c>
-      <c r="L218" s="49" t="s">
-        <v>1370</v>
       </c>
       <c r="M218" s="49"/>
       <c r="N218" s="49"/>
@@ -19108,17 +19143,17 @@
       <c r="R218" s="83"/>
       <c r="S218" s="83"/>
       <c r="T218" s="5" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="U218" s="5" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="V218" s="20"/>
       <c r="W218" s="5"/>
       <c r="X218" s="45"/>
       <c r="Y218" s="2"/>
     </row>
-    <row r="219" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A219" s="44" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -19181,7 +19216,7 @@
       </c>
       <c r="Y219" s="2"/>
     </row>
-    <row r="220" spans="1:25" ht="33" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A220" s="44" t="str">
         <f t="shared" si="20"/>
         <v>...E.05. - Other unintentional injuries</v>
@@ -19208,16 +19243,16 @@
         <v>E05</v>
       </c>
       <c r="I220" s="5" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="J220" s="5" t="s">
+        <v>1250</v>
+      </c>
+      <c r="K220" s="5" t="s">
         <v>1251</v>
       </c>
-      <c r="K220" s="5" t="s">
+      <c r="L220" s="49" t="s">
         <v>1252</v>
-      </c>
-      <c r="L220" s="49" t="s">
-        <v>1253</v>
       </c>
       <c r="M220" s="49"/>
       <c r="N220" s="49"/>
@@ -19250,7 +19285,7 @@
         <v>887</v>
       </c>
       <c r="Y220" s="22" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="221" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
@@ -19309,7 +19344,7 @@
       </c>
       <c r="Y221" s="2"/>
     </row>
-    <row r="222" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A222" s="44" t="str">
         <f t="shared" si="20"/>
         <v>...E.07. - Suicide/Self-harm</v>
@@ -19336,7 +19371,7 @@
         <v>E07</v>
       </c>
       <c r="I222" s="5" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="J222" s="5" t="s">
         <v>1210</v>
@@ -19363,10 +19398,10 @@
         <v>999</v>
       </c>
       <c r="T222" s="5" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="U222" s="5" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="V222" s="20" t="s">
         <v>140</v>
@@ -19379,7 +19414,7 @@
       </c>
       <c r="Y222" s="2"/>
     </row>
-    <row r="223" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A223" s="44" t="str">
         <f t="shared" si="20"/>
         <v>...E.08. - Homicide/Interpersonal violence</v>
@@ -19424,10 +19459,10 @@
         <v>998</v>
       </c>
       <c r="T223" s="5" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="U223" s="5" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="V223" s="20" t="s">
         <v>141</v>
@@ -19440,7 +19475,7 @@
       </c>
       <c r="Y223" s="2"/>
     </row>
-    <row r="224" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:25" ht="51" x14ac:dyDescent="0.25">
       <c r="A224" s="44" t="str">
         <f t="shared" si="20"/>
         <v>....E.08.a. - Homicide excluding legal intervention</v>
@@ -19465,14 +19500,14 @@
         <v>E08a</v>
       </c>
       <c r="I224" s="5" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="J224" s="5"/>
       <c r="K224" s="5" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="L224" s="19" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="M224" s="19"/>
       <c r="N224" s="19"/>
@@ -19482,10 +19517,10 @@
       <c r="R224" s="83"/>
       <c r="S224" s="83"/>
       <c r="T224" s="20" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="U224" s="20" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="V224" s="46"/>
       <c r="W224" s="5"/>
@@ -19517,16 +19552,16 @@
         <v>E08b</v>
       </c>
       <c r="I225" s="5" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="J225" s="5" t="s">
         <v>1210</v>
       </c>
       <c r="K225" s="5" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="L225" s="19" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="M225" s="19"/>
       <c r="N225" s="19"/>
@@ -19536,17 +19571,17 @@
       <c r="R225" s="83"/>
       <c r="S225" s="83"/>
       <c r="T225" s="20" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="U225" s="20" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="V225" s="46"/>
       <c r="W225" s="5"/>
       <c r="X225" s="45"/>
       <c r="Y225" s="2"/>
     </row>
-    <row r="226" spans="1:25" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:25" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A226" s="44" t="str">
         <f t="shared" si="20"/>
         <v>....E.08.c. - Execution, War, Terrorism</v>
@@ -19575,16 +19610,16 @@
         <v>E08c</v>
       </c>
       <c r="I226" s="5" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="J226" s="5" t="s">
         <v>1234</v>
       </c>
       <c r="K226" s="5" t="s">
+        <v>1364</v>
+      </c>
+      <c r="L226" s="49" t="s">
         <v>1365</v>
-      </c>
-      <c r="L226" s="49" t="s">
-        <v>1366</v>
       </c>
       <c r="M226" s="49"/>
       <c r="N226" s="49"/>
@@ -19598,10 +19633,10 @@
       <c r="R226" s="83"/>
       <c r="S226" s="83"/>
       <c r="T226" s="5" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="U226" s="5" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="V226" s="20" t="s">
         <v>142</v>
@@ -19616,16 +19651,16 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="227" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:25" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A227" s="44" t="str">
         <f t="shared" si="20"/>
         <v>...E.99. - Injuries of unknown intent (e.g., unintentional or self-harm), including overdoses and deaths by firearm</v>
       </c>
       <c r="B227" s="77" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="C227" s="16" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="D227" s="54" t="s">
         <v>1141</v>
@@ -19642,16 +19677,16 @@
         <v>E99</v>
       </c>
       <c r="I227" s="48" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="J227" s="48" t="s">
+        <v>1265</v>
+      </c>
+      <c r="K227" s="16" t="s">
         <v>1266</v>
       </c>
-      <c r="K227" s="16" t="s">
+      <c r="L227" s="16" t="s">
         <v>1267</v>
-      </c>
-      <c r="L227" s="16" t="s">
-        <v>1268</v>
       </c>
       <c r="T227" s="48" t="s">
         <v>1217</v>
@@ -19660,7 +19695,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="228" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:25" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A228" s="44" t="str">
         <f t="shared" si="20"/>
         <v>...Z.01. - Symptoms, signs and ill-defined conditions, not elsewhere classified</v>
@@ -19689,7 +19724,7 @@
         <v>1221</v>
       </c>
       <c r="L228" s="16" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="T228" s="48" t="s">
         <v>1222</v>
@@ -19698,7 +19733,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="229" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:25" ht="51" x14ac:dyDescent="0.25">
       <c r="A229" s="44" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -19715,7 +19750,7 @@
       </c>
       <c r="H229" s="40"/>
       <c r="I229" s="16" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="J229" s="48" t="s">
         <v>1220</v>
@@ -19733,7 +19768,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="230" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A230" s="44" t="str">
         <f t="shared" si="20"/>
         <v>...Z.02. - Unknown/Missing Value</v>
@@ -19750,13 +19785,13 @@
         <v>Z02</v>
       </c>
       <c r="T230" s="48" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="U230" s="48" t="s">
-        <v>1308</v>
-      </c>
-    </row>
-    <row r="231" spans="1:25" x14ac:dyDescent="0.25">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="231" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A231" s="44" t="str">
         <f t="shared" si="20"/>
         <v>...Z.03. - Code does not map</v>
@@ -19773,7 +19808,7 @@
         <v>Z03</v>
       </c>
       <c r="I231" s="16" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="T231" s="48" t="s">
         <v>1239</v>
@@ -19782,7 +19817,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="232" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A232" s="44" t="str">
         <f t="shared" si="20"/>
         <v>..Z. - Unknown/Missing Value</v>
@@ -19796,13 +19831,13 @@
         <v>Z</v>
       </c>
       <c r="T232" s="48" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="U232" s="48" t="s">
-        <v>1308</v>
-      </c>
-    </row>
-    <row r="233" spans="1:25" x14ac:dyDescent="0.25">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="233" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A233" s="44" t="str">
         <f t="shared" si="20"/>
         <v>...D.99. - Other Chronic Conditions</v>
@@ -19819,14 +19854,14 @@
         <v>D99</v>
       </c>
       <c r="T233" s="48" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="U233" s="48" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Y226"/>
+  <autoFilter ref="A1:Y226" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -19839,7 +19874,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20034,7 +20069,7 @@
     <row r="17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -20047,7 +20082,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C11:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20063,24 +20098,24 @@
   <sheetData>
     <row r="11" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="70" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="D11" s="71" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="E11" s="71" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="12" spans="3:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="72" t="s">
+        <v>1313</v>
+      </c>
+      <c r="D12" s="73" t="s">
         <v>1314</v>
       </c>
-      <c r="D12" s="73" t="s">
+      <c r="E12" s="73" t="s">
         <v>1315</v>
-      </c>
-      <c r="E12" s="73" t="s">
-        <v>1316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data updates - quarterly, datcounty65, etc
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/icd10_to_CAUSE.xlsx
+++ b/myCBD/myInfo/icd10_to_CAUSE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\CCB\CCB Project\0.CCB\myCBD\myInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A38315-AC94-42C4-B678-4CCF0CA5476D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D34C96A-99FD-4048-B2CB-C491B23AC2E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3315" yWindow="780" windowWidth="21840" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3097" uniqueCount="1426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3097" uniqueCount="1428">
   <si>
     <t>I. Communicable, maternal, perinatal and nutritional conditions</t>
   </si>
@@ -4560,6 +4560,12 @@
   </si>
   <si>
     <t>H3[0-4]|\\bH35\\b|H35[0-2,4-9]|H5[3-4]</t>
+  </si>
+  <si>
+    <t>B16-B19 (minus B17.1, B17.2, B17.8, B18.2, B18.8)</t>
+  </si>
+  <si>
+    <t>B16|B17[0,3-7,9]|B18[0-1,3-7,9]|B19</t>
   </si>
 </sst>
 </file>
@@ -5531,10 +5537,10 @@
   <dimension ref="A1:Y233"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B137" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L155" sqref="L155"/>
+      <selection pane="bottomRight" activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7157,10 +7163,10 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5" t="s">
-        <v>962</v>
+        <v>1426</v>
       </c>
       <c r="L27" s="16" t="s">
-        <v>341</v>
+        <v>1427</v>
       </c>
       <c r="O27" s="59" t="s">
         <v>962</v>

</xml_diff>